<commit_message>
revert: to use edeg implementation
</commit_message>
<xml_diff>
--- a/cognite/neat/_rules/catalog/classic_model.xlsx
+++ b/cognite/neat/_rules/catalog/classic_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\cognite\neat\_rules\catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAB7257-450F-4675-8945-6AE9821767D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA047A8-9571-4215-AB42-DFAA26B27217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="82">
   <si>
     <t>role</t>
   </si>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t>Instance Source</t>
+  </si>
+  <si>
+    <t>Edge</t>
   </si>
 </sst>
 </file>
@@ -773,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I42" sqref="I42"/>
     </sheetView>
@@ -2331,9 +2334,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2395,6 +2398,9 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>62</v>
+      </c>
+      <c r="D7" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix; bug in core model
</commit_message>
<xml_diff>
--- a/cognite/neat/_rules/catalog/classic_model.xlsx
+++ b/cognite/neat/_rules/catalog/classic_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\cognite\neat\_rules\catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA047A8-9571-4215-AB42-DFAA26B27217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCCA931-51D9-452A-A41D-013E33C61100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -776,9 +776,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,7 +2028,7 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="7">
@@ -2334,7 +2334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>

</xml_diff>

<commit_message>
refactor; remove implements edge from relationship
</commit_message>
<xml_diff>
--- a/cognite/neat/_rules/catalog/classic_model.xlsx
+++ b/cognite/neat/_rules/catalog/classic_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\cognite\neat\_rules\catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCCA931-51D9-452A-A41D-013E33C61100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8980EDDD-A8E4-4DA1-A92C-66CD45ABE8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="3840" windowWidth="30960" windowHeight="12120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="81">
   <si>
     <t>role</t>
   </si>
@@ -266,9 +266,6 @@
   </si>
   <si>
     <t>Instance Source</t>
-  </si>
-  <si>
-    <t>Edge</t>
   </si>
 </sst>
 </file>
@@ -679,13 +676,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -701,7 +698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -709,7 +706,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -717,7 +714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -725,7 +722,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -733,7 +730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -741,7 +738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -749,7 +746,7 @@
         <v>45665.278279401493</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -757,12 +754,12 @@
         <v>45665.278279401493</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -776,23 +773,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
     <col min="6" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="45.42578125" customWidth="1"/>
+    <col min="9" max="9" width="45.44140625" customWidth="1"/>
     <col min="10" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -807,7 +804,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -842,7 +839,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>59</v>
       </c>
@@ -863,7 +860,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>59</v>
       </c>
@@ -884,7 +881,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>59</v>
       </c>
@@ -905,7 +902,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>59</v>
       </c>
@@ -926,7 +923,7 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>59</v>
       </c>
@@ -947,7 +944,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>59</v>
       </c>
@@ -968,7 +965,7 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>59</v>
       </c>
@@ -989,7 +986,7 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>59</v>
       </c>
@@ -1010,7 +1007,7 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>59</v>
       </c>
@@ -1031,7 +1028,7 @@
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>60</v>
       </c>
@@ -1052,7 +1049,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>60</v>
       </c>
@@ -1073,7 +1070,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>60</v>
       </c>
@@ -1094,7 +1091,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>60</v>
       </c>
@@ -1115,7 +1112,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>60</v>
       </c>
@@ -1136,7 +1133,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>60</v>
       </c>
@@ -1157,7 +1154,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>60</v>
       </c>
@@ -1178,7 +1175,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>60</v>
       </c>
@@ -1199,7 +1196,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>60</v>
       </c>
@@ -1220,7 +1217,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>60</v>
       </c>
@@ -1241,7 +1238,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>62</v>
       </c>
@@ -1262,7 +1259,7 @@
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>62</v>
       </c>
@@ -1283,7 +1280,7 @@
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>62</v>
       </c>
@@ -1304,7 +1301,7 @@
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>62</v>
       </c>
@@ -1325,7 +1322,7 @@
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>62</v>
       </c>
@@ -1346,7 +1343,7 @@
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>62</v>
       </c>
@@ -1367,7 +1364,7 @@
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>62</v>
       </c>
@@ -1388,7 +1385,7 @@
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>62</v>
       </c>
@@ -1409,7 +1406,7 @@
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>62</v>
       </c>
@@ -1430,7 +1427,7 @@
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>62</v>
       </c>
@@ -1451,7 +1448,7 @@
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>61</v>
       </c>
@@ -1472,7 +1469,7 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>61</v>
       </c>
@@ -1493,7 +1490,7 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>61</v>
       </c>
@@ -1514,7 +1511,7 @@
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>61</v>
       </c>
@@ -1535,7 +1532,7 @@
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>61</v>
       </c>
@@ -1556,7 +1553,7 @@
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>61</v>
       </c>
@@ -1577,7 +1574,7 @@
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>61</v>
       </c>
@@ -1598,7 +1595,7 @@
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>61</v>
       </c>
@@ -1619,7 +1616,7 @@
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>61</v>
       </c>
@@ -1640,7 +1637,7 @@
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>61</v>
       </c>
@@ -1661,7 +1658,7 @@
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>61</v>
       </c>
@@ -1682,7 +1679,7 @@
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>61</v>
       </c>
@@ -1703,7 +1700,7 @@
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>61</v>
       </c>
@@ -1724,7 +1721,7 @@
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>58</v>
       </c>
@@ -1745,7 +1742,7 @@
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>58</v>
       </c>
@@ -1766,7 +1763,7 @@
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>58</v>
       </c>
@@ -1787,7 +1784,7 @@
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>58</v>
       </c>
@@ -1808,7 +1805,7 @@
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>58</v>
       </c>
@@ -1829,7 +1826,7 @@
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>58</v>
       </c>
@@ -1850,7 +1847,7 @@
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>58</v>
       </c>
@@ -1871,7 +1868,7 @@
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>58</v>
       </c>
@@ -1892,7 +1889,7 @@
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>58</v>
       </c>
@@ -1913,7 +1910,7 @@
       <c r="J53" s="7"/>
       <c r="K53" s="7"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>58</v>
       </c>
@@ -1934,7 +1931,7 @@
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>58</v>
       </c>
@@ -1955,7 +1952,7 @@
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>72</v>
       </c>
@@ -1976,7 +1973,7 @@
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>72</v>
       </c>
@@ -1997,7 +1994,7 @@
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>72</v>
       </c>
@@ -2018,7 +2015,7 @@
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>72</v>
       </c>
@@ -2039,7 +2036,7 @@
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>72</v>
       </c>
@@ -2060,7 +2057,7 @@
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
         <v>63</v>
       </c>
@@ -2081,7 +2078,7 @@
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>63</v>
       </c>
@@ -2102,7 +2099,7 @@
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>63</v>
       </c>
@@ -2123,7 +2120,7 @@
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
         <v>63</v>
       </c>
@@ -2144,7 +2141,7 @@
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>75</v>
       </c>
@@ -2165,7 +2162,7 @@
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>75</v>
       </c>
@@ -2186,7 +2183,7 @@
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>75</v>
       </c>
@@ -2207,7 +2204,7 @@
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
         <v>75</v>
       </c>
@@ -2228,7 +2225,7 @@
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
         <v>75</v>
       </c>
@@ -2249,7 +2246,7 @@
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
         <v>75</v>
       </c>
@@ -2270,7 +2267,7 @@
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>75</v>
       </c>
@@ -2291,7 +2288,7 @@
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>75</v>
       </c>
@@ -2312,7 +2309,7 @@
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -2334,18 +2331,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
     <col min="2" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>49</v>
       </c>
@@ -2355,7 +2352,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -2375,45 +2372,42 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>62</v>
       </c>
-      <c r="D7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -2429,13 +2423,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="36.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -2443,7 +2437,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -2451,7 +2445,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
[NEAT-697] 🚵 Edge change (#912)
* refactor; classic rules

* refactor: moved model to catalog

* refactor; implemented information rules

* refactor; fix

* Ãrefactor:

* refactor: prepare core

* refactor: renaming

* refactor setup transformations

* fix; adding prefix

* fix: reading source

* refactor: fix graph reading

* refactor; regen

* refactor: added missing description

* revert: to use edeg implementation

* fix; bug in core model

* tests; regen

* fix: Information class

* fix: bug reading datasets

* fix: self inflicted pain

* tests; regen

* fix: added parser

* tests: update test

* tests: update test

* refactor: edge recognized by start and end node

* refactor: smart container conversoin

* build: changelog

* fix: update specialized

* refactor; remove implements edge from relationship

* tests: regen

* tests: regen

* tests: skip offending test

* feat: first pass relationship lookup transformer

* refactor: include lookup

* fix: bugs in transformation lookup
</commit_message>
<xml_diff>
--- a/cognite/neat/_rules/catalog/classic_model.xlsx
+++ b/cognite/neat/_rules/catalog/classic_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\cognite\neat\_rules\catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCCA931-51D9-452A-A41D-013E33C61100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8980EDDD-A8E4-4DA1-A92C-66CD45ABE8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="3840" windowWidth="30960" windowHeight="12120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="81">
   <si>
     <t>role</t>
   </si>
@@ -266,9 +266,6 @@
   </si>
   <si>
     <t>Instance Source</t>
-  </si>
-  <si>
-    <t>Edge</t>
   </si>
 </sst>
 </file>
@@ -679,13 +676,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -701,7 +698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -709,7 +706,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -717,7 +714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -725,7 +722,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -733,7 +730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -741,7 +738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -749,7 +746,7 @@
         <v>45665.278279401493</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -757,12 +754,12 @@
         <v>45665.278279401493</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -776,23 +773,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
     <col min="6" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="45.42578125" customWidth="1"/>
+    <col min="9" max="9" width="45.44140625" customWidth="1"/>
     <col min="10" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -807,7 +804,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -842,7 +839,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>59</v>
       </c>
@@ -863,7 +860,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>59</v>
       </c>
@@ -884,7 +881,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>59</v>
       </c>
@@ -905,7 +902,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>59</v>
       </c>
@@ -926,7 +923,7 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>59</v>
       </c>
@@ -947,7 +944,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>59</v>
       </c>
@@ -968,7 +965,7 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>59</v>
       </c>
@@ -989,7 +986,7 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>59</v>
       </c>
@@ -1010,7 +1007,7 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>59</v>
       </c>
@@ -1031,7 +1028,7 @@
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>60</v>
       </c>
@@ -1052,7 +1049,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>60</v>
       </c>
@@ -1073,7 +1070,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>60</v>
       </c>
@@ -1094,7 +1091,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>60</v>
       </c>
@@ -1115,7 +1112,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>60</v>
       </c>
@@ -1136,7 +1133,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>60</v>
       </c>
@@ -1157,7 +1154,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>60</v>
       </c>
@@ -1178,7 +1175,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>60</v>
       </c>
@@ -1199,7 +1196,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>60</v>
       </c>
@@ -1220,7 +1217,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>60</v>
       </c>
@@ -1241,7 +1238,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>62</v>
       </c>
@@ -1262,7 +1259,7 @@
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>62</v>
       </c>
@@ -1283,7 +1280,7 @@
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>62</v>
       </c>
@@ -1304,7 +1301,7 @@
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>62</v>
       </c>
@@ -1325,7 +1322,7 @@
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>62</v>
       </c>
@@ -1346,7 +1343,7 @@
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>62</v>
       </c>
@@ -1367,7 +1364,7 @@
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>62</v>
       </c>
@@ -1388,7 +1385,7 @@
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>62</v>
       </c>
@@ -1409,7 +1406,7 @@
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>62</v>
       </c>
@@ -1430,7 +1427,7 @@
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>62</v>
       </c>
@@ -1451,7 +1448,7 @@
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>61</v>
       </c>
@@ -1472,7 +1469,7 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>61</v>
       </c>
@@ -1493,7 +1490,7 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>61</v>
       </c>
@@ -1514,7 +1511,7 @@
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>61</v>
       </c>
@@ -1535,7 +1532,7 @@
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>61</v>
       </c>
@@ -1556,7 +1553,7 @@
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>61</v>
       </c>
@@ -1577,7 +1574,7 @@
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>61</v>
       </c>
@@ -1598,7 +1595,7 @@
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>61</v>
       </c>
@@ -1619,7 +1616,7 @@
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>61</v>
       </c>
@@ -1640,7 +1637,7 @@
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>61</v>
       </c>
@@ -1661,7 +1658,7 @@
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>61</v>
       </c>
@@ -1682,7 +1679,7 @@
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>61</v>
       </c>
@@ -1703,7 +1700,7 @@
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>61</v>
       </c>
@@ -1724,7 +1721,7 @@
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>58</v>
       </c>
@@ -1745,7 +1742,7 @@
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>58</v>
       </c>
@@ -1766,7 +1763,7 @@
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>58</v>
       </c>
@@ -1787,7 +1784,7 @@
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>58</v>
       </c>
@@ -1808,7 +1805,7 @@
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>58</v>
       </c>
@@ -1829,7 +1826,7 @@
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>58</v>
       </c>
@@ -1850,7 +1847,7 @@
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>58</v>
       </c>
@@ -1871,7 +1868,7 @@
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>58</v>
       </c>
@@ -1892,7 +1889,7 @@
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>58</v>
       </c>
@@ -1913,7 +1910,7 @@
       <c r="J53" s="7"/>
       <c r="K53" s="7"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>58</v>
       </c>
@@ -1934,7 +1931,7 @@
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>58</v>
       </c>
@@ -1955,7 +1952,7 @@
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>72</v>
       </c>
@@ -1976,7 +1973,7 @@
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>72</v>
       </c>
@@ -1997,7 +1994,7 @@
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>72</v>
       </c>
@@ -2018,7 +2015,7 @@
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>72</v>
       </c>
@@ -2039,7 +2036,7 @@
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>72</v>
       </c>
@@ -2060,7 +2057,7 @@
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
         <v>63</v>
       </c>
@@ -2081,7 +2078,7 @@
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>63</v>
       </c>
@@ -2102,7 +2099,7 @@
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>63</v>
       </c>
@@ -2123,7 +2120,7 @@
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
         <v>63</v>
       </c>
@@ -2144,7 +2141,7 @@
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>75</v>
       </c>
@@ -2165,7 +2162,7 @@
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>75</v>
       </c>
@@ -2186,7 +2183,7 @@
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>75</v>
       </c>
@@ -2207,7 +2204,7 @@
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
         <v>75</v>
       </c>
@@ -2228,7 +2225,7 @@
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
         <v>75</v>
       </c>
@@ -2249,7 +2246,7 @@
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
         <v>75</v>
       </c>
@@ -2270,7 +2267,7 @@
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>75</v>
       </c>
@@ -2291,7 +2288,7 @@
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>75</v>
       </c>
@@ -2312,7 +2309,7 @@
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -2334,18 +2331,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
     <col min="2" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>49</v>
       </c>
@@ -2355,7 +2352,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -2375,45 +2372,42 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>62</v>
       </c>
-      <c r="D7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -2429,13 +2423,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="36.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -2443,7 +2437,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -2451,7 +2445,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
refactor; update metdata classic
</commit_message>
<xml_diff>
--- a/cognite/neat/_rules/catalog/classic_model.xlsx
+++ b/cognite/neat/_rules/catalog/classic_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\cognite\neat\_rules\catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8980EDDD-A8E4-4DA1-A92C-66CD45ABE8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB7BA09-3520-4B27-B8C4-EE45F61C6266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="3840" windowWidth="30960" windowHeight="12120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="80">
   <si>
     <t>role</t>
   </si>
@@ -49,21 +49,12 @@
     <t>name</t>
   </si>
   <si>
-    <t>Inferred Model</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
-    <t>Inferred model from knowledge graph</t>
-  </si>
-  <si>
     <t>creator</t>
   </si>
   <si>
-    <t>NEAT</t>
-  </si>
-  <si>
     <t>created</t>
   </si>
   <si>
@@ -266,6 +257,12 @@
   </si>
   <si>
     <t>Instance Source</t>
+  </si>
+  <si>
+    <t>The data model matching the classic model in CDF</t>
+  </si>
+  <si>
+    <t>Cognite</t>
   </si>
 </sst>
 </file>
@@ -672,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,7 +700,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -719,28 +716,28 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2">
         <v>45665.278279401493</v>
@@ -748,7 +745,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2">
         <v>45665.278279401493</v>
@@ -756,12 +753,12 @@
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -791,7 +788,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -806,50 +803,50 @@
     </row>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="I2" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6">
@@ -862,15 +859,15 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6">
@@ -883,15 +880,15 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6">
@@ -904,7 +901,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>7</v>
@@ -912,7 +909,7 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6">
@@ -925,15 +922,15 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6">
@@ -946,15 +943,15 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6">
@@ -967,15 +964,15 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6">
@@ -988,7 +985,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>4</v>
@@ -996,7 +993,7 @@
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6">
@@ -1009,15 +1006,15 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6">
@@ -1030,15 +1027,15 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7">
@@ -1051,7 +1048,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>4</v>
@@ -1059,7 +1056,7 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7">
@@ -1072,15 +1069,15 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7">
@@ -1093,15 +1090,15 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7">
@@ -1114,15 +1111,15 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7">
@@ -1135,15 +1132,15 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7">
@@ -1156,15 +1153,15 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7">
@@ -1177,15 +1174,15 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7">
@@ -1198,15 +1195,15 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7">
@@ -1219,15 +1216,15 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7">
@@ -1240,15 +1237,15 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6">
@@ -1261,15 +1258,15 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6">
@@ -1282,15 +1279,15 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6">
@@ -1303,7 +1300,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>4</v>
@@ -1311,7 +1308,7 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6">
@@ -1324,15 +1321,15 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6">
@@ -1345,15 +1342,15 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6">
@@ -1366,15 +1363,15 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6">
@@ -1387,15 +1384,15 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6">
@@ -1408,15 +1405,15 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6">
@@ -1429,15 +1426,15 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6">
@@ -1450,15 +1447,15 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7">
@@ -1471,15 +1468,15 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="7">
@@ -1492,15 +1489,15 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7">
@@ -1513,15 +1510,15 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="7">
@@ -1534,7 +1531,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>4</v>
@@ -1542,7 +1539,7 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7">
@@ -1555,7 +1552,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>7</v>
@@ -1563,7 +1560,7 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="7">
@@ -1576,15 +1573,15 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="7">
@@ -1597,15 +1594,15 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7">
@@ -1618,15 +1615,15 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="7">
@@ -1639,15 +1636,15 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="7">
@@ -1660,15 +1657,15 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="7">
@@ -1681,15 +1678,15 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="7">
@@ -1702,15 +1699,15 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="7">
@@ -1723,7 +1720,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>4</v>
@@ -1731,7 +1728,7 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="7">
@@ -1744,15 +1741,15 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="7">
@@ -1765,15 +1762,15 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="7">
@@ -1786,15 +1783,15 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="7">
@@ -1807,15 +1804,15 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F49" s="7"/>
       <c r="G49" s="7">
@@ -1828,15 +1825,15 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="7">
@@ -1849,15 +1846,15 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="7">
@@ -1870,15 +1867,15 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="7">
@@ -1891,7 +1888,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>7</v>
@@ -1899,7 +1896,7 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F53" s="7"/>
       <c r="G53" s="7">
@@ -1912,15 +1909,15 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="7">
@@ -1933,15 +1930,15 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="7">
@@ -1954,7 +1951,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>4</v>
@@ -1962,7 +1959,7 @@
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F56" s="7"/>
       <c r="G56" s="7">
@@ -1975,7 +1972,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>7</v>
@@ -1983,7 +1980,7 @@
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="7">
@@ -1996,15 +1993,15 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="7">
@@ -2017,15 +2014,15 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="7">
@@ -2038,15 +2035,15 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="7">
@@ -2059,7 +2056,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>4</v>
@@ -2067,7 +2064,7 @@
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
       <c r="E61" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="7">
@@ -2080,7 +2077,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>7</v>
@@ -2088,7 +2085,7 @@
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
       <c r="E62" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F62" s="9"/>
       <c r="G62" s="7">
@@ -2101,15 +2098,15 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
       <c r="E63" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F63" s="9"/>
       <c r="G63" s="7">
@@ -2122,15 +2119,15 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
       <c r="E64" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F64" s="9"/>
       <c r="G64" s="9">
@@ -2143,7 +2140,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>4</v>
@@ -2151,7 +2148,7 @@
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
       <c r="E65" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F65" s="9"/>
       <c r="G65" s="7">
@@ -2164,7 +2161,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>7</v>
@@ -2172,7 +2169,7 @@
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
       <c r="E66" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F66" s="9"/>
       <c r="G66" s="7">
@@ -2185,15 +2182,15 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C67" s="9"/>
       <c r="D67" s="9"/>
       <c r="E67" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F67" s="9"/>
       <c r="G67" s="9">
@@ -2206,15 +2203,15 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
       <c r="E68" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F68" s="9"/>
       <c r="G68" s="7">
@@ -2227,15 +2224,15 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
       <c r="E69" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F69" s="9"/>
       <c r="G69" s="9">
@@ -2248,15 +2245,15 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
       <c r="E70" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F70" s="9"/>
       <c r="G70" s="9">
@@ -2269,15 +2266,15 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
       <c r="E71" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F71" s="9"/>
       <c r="G71" s="9">
@@ -2290,15 +2287,15 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
       <c r="E72" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F72" s="9"/>
       <c r="G72" s="9">
@@ -2331,7 +2328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
@@ -2344,7 +2341,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2354,62 +2351,62 @@
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2431,26 +2428,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>